<commit_message>
(+) import bappeda function
</commit_message>
<xml_diff>
--- a/public/others/Format Import Dosen - KKN UNDIP.xlsx
+++ b/public/others/Format Import Dosen - KKN UNDIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Skripsi\kkn-undip-fe\public\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AB3BAD-5D26-4C64-8918-6B7E02FADF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565214B3-CFF6-4B94-9309-1E7E8374CA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3AE134CB-FC35-47DF-B16F-B4C1D76A39BA}"/>
   </bookViews>
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -123,6 +123,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CCC9AD-8811-4329-B6C0-75514A096BDC}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -475,59 +480,769 @@
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="9"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="9"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="9"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="9"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="9"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="9"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="9"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="7"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="9"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="9"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="9"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="7"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="9"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="7"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="9"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="7"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="9"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="7"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="9"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="7"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="7"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="9"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="7"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="9"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="7"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="9"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="7"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="9"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="7"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="9"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="7"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="9"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="7"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="9"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="7"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="9"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="7"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="9"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="7"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="9"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="7"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="9"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="7"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="9"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="7"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="9"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="7"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="9"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="7"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="9"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="7"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="9"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="7"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="9"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="7"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="9"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="7"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="9"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="7"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="9"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="7"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="9"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="7"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="9"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="7"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="9"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="7"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="9"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="7"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="9"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="7"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="9"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="7"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="9"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="7"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="9"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="7"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="9"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="7"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="9"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="7"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="9"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="7"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="9"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="7"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="9"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="7"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="9"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="7"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="9"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="7"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="9"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="7"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="9"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="7"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="9"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="7"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="9"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="7"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="9"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="7"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="9"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="7"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="9"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="7"/>
+      <c r="B97" s="8"/>
+      <c r="C97" s="9"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="7"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="9"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="7"/>
+      <c r="B99" s="8"/>
+      <c r="C99" s="9"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="7"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="9"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="7"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="9"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="7"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="9"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="7"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="9"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="7"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="9"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="7"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="9"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="7"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="9"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="7"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="9"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="7"/>
+      <c r="B108" s="8"/>
+      <c r="C108" s="9"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="7"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="9"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="7"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="9"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="7"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="9"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="7"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="9"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="7"/>
+      <c r="B113" s="8"/>
+      <c r="C113" s="9"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="7"/>
+      <c r="B114" s="8"/>
+      <c r="C114" s="9"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="7"/>
+      <c r="B115" s="8"/>
+      <c r="C115" s="9"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="7"/>
+      <c r="B116" s="8"/>
+      <c r="C116" s="9"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="7"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="9"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="7"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="9"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="7"/>
+      <c r="B119" s="8"/>
+      <c r="C119" s="9"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="7"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="9"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="7"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="9"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="7"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="9"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="7"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="9"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="7"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="9"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="7"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="9"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="7"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="9"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="7"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="9"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="7"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="9"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="7"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="9"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="7"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="9"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="7"/>
+      <c r="B131" s="8"/>
+      <c r="C131" s="9"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="7"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="9"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="7"/>
+      <c r="B133" s="8"/>
+      <c r="C133" s="9"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="7"/>
+      <c r="B134" s="8"/>
+      <c r="C134" s="9"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="7"/>
+      <c r="B135" s="8"/>
+      <c r="C135" s="9"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="7"/>
+      <c r="B136" s="8"/>
+      <c r="C136" s="9"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="7"/>
+      <c r="B137" s="8"/>
+      <c r="C137" s="9"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="7"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="9"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" s="7"/>
+      <c r="B139" s="8"/>
+      <c r="C139" s="9"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" s="7"/>
+      <c r="B140" s="8"/>
+      <c r="C140" s="9"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" s="7"/>
+      <c r="B141" s="8"/>
+      <c r="C141" s="9"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="7"/>
+      <c r="B142" s="8"/>
+      <c r="C142" s="9"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" s="7"/>
+      <c r="B143" s="8"/>
+      <c r="C143" s="9"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="7"/>
+      <c r="B144" s="8"/>
+      <c r="C144" s="9"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" s="7"/>
+      <c r="B145" s="8"/>
+      <c r="C145" s="9"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" s="7"/>
+      <c r="B146" s="8"/>
+      <c r="C146" s="9"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" s="7"/>
+      <c r="B147" s="8"/>
+      <c r="C147" s="9"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="7"/>
+      <c r="B148" s="8"/>
+      <c r="C148" s="9"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" s="7"/>
+      <c r="B149" s="8"/>
+      <c r="C149" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">

</xml_diff>